<commit_message>
Fixed Bom issue with C12 and C14
Fixed Bom issue with C12 and C14
</commit_message>
<xml_diff>
--- a/SoundNicer BOM.xlsx
+++ b/SoundNicer BOM.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oren\Desktop\SoundNicer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="945" yWindow="0" windowWidth="17280" windowHeight="8775"/>
   </bookViews>
@@ -144,9 +149,6 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>CAP 0.5pF 25V ±0.1pF 0805 (2012 Metric) Thickness 0.75mm SMD</t>
-  </si>
-  <si>
     <t>C12, C14</t>
   </si>
   <si>
@@ -295,6 +297,9 @@
   </si>
   <si>
     <t>50k</t>
+  </si>
+  <si>
+    <t>100nF 0805</t>
   </si>
 </sst>
 </file>
@@ -680,15 +685,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.53125" customWidth="1"/>
-    <col min="7" max="8" width="6.73046875" customWidth="1"/>
+    <col min="1" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -740,7 +747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -766,7 +773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -792,7 +799,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -818,7 +825,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -844,7 +851,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -870,7 +877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -896,21 +903,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
@@ -922,38 +929,38 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>27</v>
@@ -968,18 +975,18 @@
         <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
@@ -994,200 +1001,200 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F13" s="3">
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="F19" s="3">
         <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>27</v>
@@ -1202,18 +1209,18 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>27</v>
@@ -1228,18 +1235,18 @@
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>27</v>
@@ -1254,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>27</v>

</xml_diff>